<commit_message>
add last 4 ashing values for samples 37-40
</commit_message>
<xml_diff>
--- a/02_Data/03_Scale/Gravimetric_analysis.xlsx
+++ b/02_Data/03_Scale/Gravimetric_analysis.xlsx
@@ -324,7 +324,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+      <selection pane="topLeft" activeCell="N34" activeCellId="0" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1480,6 +1480,9 @@
       <c r="D38" s="1" t="n">
         <v>0.5477</v>
       </c>
+      <c r="E38" s="1" t="n">
+        <v>0.3448</v>
+      </c>
       <c r="F38" s="1" t="n">
         <v>0.2901</v>
       </c>
@@ -1507,6 +1510,9 @@
       <c r="D39" s="1" t="n">
         <v>0.5079</v>
       </c>
+      <c r="E39" s="1" t="n">
+        <v>0.3157</v>
+      </c>
       <c r="F39" s="1" t="n">
         <v>0.2674</v>
       </c>
@@ -1537,6 +1543,9 @@
       <c r="D40" s="1" t="n">
         <v>0.5687</v>
       </c>
+      <c r="E40" s="1" t="n">
+        <v>0.3504</v>
+      </c>
       <c r="F40" s="1" t="n">
         <v>0.2975</v>
       </c>
@@ -1563,6 +1572,9 @@
       </c>
       <c r="D41" s="1" t="n">
         <v>0.4797</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>0.2955</v>
       </c>
       <c r="F41" s="1" t="n">
         <v>0.2488</v>

</xml_diff>

<commit_message>
adapted to take full sample set into account (76 samples)
</commit_message>
<xml_diff>
--- a/02_Data/03_Scale/Gravimetric_analysis.xlsx
+++ b/02_Data/03_Scale/Gravimetric_analysis.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="95">
   <si>
     <t xml:space="preserve">Sample Nr</t>
   </si>
@@ -49,15 +49,18 @@
     <t xml:space="preserve">notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Density</t>
-  </si>
-  <si>
     <t xml:space="preserve">age</t>
   </si>
   <si>
+    <t xml:space="preserve">sex</t>
+  </si>
+  <si>
     <t xml:space="preserve">385_L</t>
   </si>
   <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
     <t xml:space="preserve">385_R</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t xml:space="preserve">388_L</t>
   </si>
   <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
     <t xml:space="preserve">388_R</t>
   </si>
   <si>
@@ -118,7 +124,7 @@
     <t xml:space="preserve">399_R</t>
   </si>
   <si>
-    <t xml:space="preserve">400_l</t>
+    <t xml:space="preserve">400_L</t>
   </si>
   <si>
     <t xml:space="preserve">400_R</t>
@@ -308,12 +314,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -395,7 +400,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -404,11 +409,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -417,10 +422,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -441,27 +442,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:AY81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G43" activeCellId="0" sqref="G43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="8.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="3" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="13" style="2" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,7 +490,7 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -518,24 +519,21 @@
       <c r="G2" s="1" t="n">
         <v>2997</v>
       </c>
-      <c r="I2" s="2" t="n">
-        <f aca="false">C2*$K$2/(C2-F2)</f>
-        <v>1.91338788527989</v>
-      </c>
-      <c r="J2" s="4" t="n">
+      <c r="I2" s="3" t="n">
         <v>87</v>
       </c>
-      <c r="K2" s="1" t="n">
-        <v>0.99754</v>
-      </c>
-      <c r="L2" s="5"/>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0.5426</v>
@@ -552,21 +550,19 @@
       <c r="G3" s="1" t="n">
         <v>2998</v>
       </c>
-      <c r="I3" s="2" t="n">
-        <f aca="false">C3*$K$2/(C3-F3)</f>
-        <v>1.94141034433286</v>
-      </c>
-      <c r="J3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="J3" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0.6119</v>
@@ -583,12 +579,11 @@
       <c r="G4" s="1" t="n">
         <v>2999</v>
       </c>
-      <c r="I4" s="2" t="n">
-        <f aca="false">C4*$K$2/(C4-F4)</f>
-        <v>1.97987261109309</v>
-      </c>
-      <c r="J4" s="1" t="n">
+      <c r="I4" s="1" t="n">
         <v>76</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,7 +591,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0.5484</v>
@@ -613,12 +608,11 @@
       <c r="G5" s="1" t="n">
         <v>3000</v>
       </c>
-      <c r="I5" s="2" t="n">
-        <f aca="false">C5*$K$2/(C5-F5)</f>
-        <v>1.93989693617021</v>
-      </c>
-      <c r="J5" s="1" t="n">
+      <c r="I5" s="1" t="n">
         <v>81</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -626,7 +620,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0.5622</v>
@@ -643,12 +637,11 @@
       <c r="G6" s="1" t="n">
         <v>3001</v>
       </c>
-      <c r="I6" s="2" t="n">
-        <f aca="false">C6*$K$2/(C6-F6)</f>
-        <v>1.97679586887557</v>
-      </c>
-      <c r="J6" s="1" t="n">
+      <c r="I6" s="1" t="n">
         <v>88</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,7 +649,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0.5647</v>
@@ -673,12 +666,11 @@
       <c r="G7" s="1" t="n">
         <v>3002</v>
       </c>
-      <c r="I7" s="2" t="n">
-        <f aca="false">C7*$K$2/(C7-F7)</f>
-        <v>1.98628645275035</v>
-      </c>
-      <c r="J7" s="1" t="n">
+      <c r="I7" s="1" t="n">
         <v>88</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,7 +678,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.5565</v>
@@ -703,12 +695,11 @@
       <c r="G8" s="1" t="n">
         <v>3003</v>
       </c>
-      <c r="I8" s="2" t="n">
-        <f aca="false">C8*$K$2/(C8-F8)</f>
-        <v>2.0048068255688</v>
-      </c>
-      <c r="J8" s="1" t="n">
+      <c r="I8" s="1" t="n">
         <v>91</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,7 +707,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0.5834</v>
@@ -733,12 +724,11 @@
       <c r="G9" s="1" t="n">
         <v>3004</v>
       </c>
-      <c r="I9" s="2" t="n">
-        <f aca="false">C9*$K$2/(C9-F9)</f>
-        <v>2.00125459422283</v>
-      </c>
-      <c r="J9" s="1" t="n">
+      <c r="I9" s="1" t="n">
         <v>91</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,7 +736,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0.4961</v>
@@ -761,14 +751,13 @@
         <v>0.2127</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <f aca="false">C10*$K$2/(C10-F10)</f>
-        <v>1.74622298517996</v>
-      </c>
-      <c r="J10" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="I10" s="1" t="n">
         <v>96</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,7 +765,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0.5625</v>
@@ -793,12 +782,11 @@
       <c r="G11" s="1" t="n">
         <v>3005</v>
       </c>
-      <c r="I11" s="2" t="n">
-        <f aca="false">C11*$K$2/(C11-F11)</f>
-        <v>1.94090712556209</v>
-      </c>
-      <c r="J11" s="1" t="n">
+      <c r="I11" s="1" t="n">
         <v>94</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,7 +794,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0.5694</v>
@@ -823,12 +811,11 @@
       <c r="G12" s="1" t="n">
         <v>3006</v>
       </c>
-      <c r="I12" s="2" t="n">
-        <f aca="false">C12*$K$2/(C12-F12)</f>
-        <v>1.94453706264978</v>
-      </c>
-      <c r="J12" s="1" t="n">
+      <c r="I12" s="1" t="n">
         <v>94</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,7 +823,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.5793</v>
@@ -853,12 +840,11 @@
       <c r="G13" s="1" t="n">
         <v>3007</v>
       </c>
-      <c r="I13" s="2" t="n">
-        <f aca="false">C13*$K$2/(C13-F13)</f>
-        <v>1.93333864837738</v>
-      </c>
-      <c r="J13" s="1" t="n">
+      <c r="I13" s="1" t="n">
         <v>78</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,9 +852,9 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="n">
         <v>0.538</v>
       </c>
       <c r="D14" s="1" t="n">
@@ -883,12 +869,11 @@
       <c r="G14" s="1" t="n">
         <v>3008</v>
       </c>
-      <c r="I14" s="2" t="n">
-        <f aca="false">C14*$K$2/(C14-F14)</f>
-        <v>1.92013066189624</v>
-      </c>
-      <c r="J14" s="1" t="n">
+      <c r="I14" s="1" t="n">
         <v>78</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,7 +881,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0.5547</v>
@@ -913,12 +898,11 @@
       <c r="G15" s="1" t="n">
         <v>3009</v>
       </c>
-      <c r="I15" s="2" t="n">
-        <f aca="false">C15*$K$2/(C15-F15)</f>
-        <v>1.91863882801664</v>
-      </c>
-      <c r="J15" s="1" t="n">
+      <c r="I15" s="1" t="n">
         <v>91</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,7 +910,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.4772</v>
@@ -941,14 +925,13 @@
         <v>0.2224</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="2" t="n">
-        <f aca="false">C16*$K$2/(C16-F16)</f>
-        <v>1.86823425431711</v>
-      </c>
-      <c r="J16" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="I16" s="1" t="n">
         <v>91</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,7 +939,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.5973</v>
@@ -973,12 +956,11 @@
       <c r="G17" s="1" t="n">
         <v>3010</v>
       </c>
-      <c r="I17" s="2" t="n">
-        <f aca="false">C17*$K$2/(C17-F17)</f>
-        <v>1.99809068410463</v>
-      </c>
-      <c r="J17" s="1" t="n">
+      <c r="I17" s="1" t="n">
         <v>64</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,7 +968,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0.6042</v>
@@ -1003,12 +985,11 @@
       <c r="G18" s="1" t="n">
         <v>3011</v>
       </c>
-      <c r="I18" s="2" t="n">
-        <f aca="false">C18*$K$2/(C18-F18)</f>
-        <v>1.98915401980198</v>
-      </c>
-      <c r="J18" s="1" t="n">
+      <c r="I18" s="1" t="n">
         <v>64</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,7 +997,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0.5666</v>
@@ -1033,12 +1014,11 @@
       <c r="G19" s="1" t="n">
         <v>3012</v>
       </c>
-      <c r="I19" s="2" t="n">
-        <f aca="false">C19*$K$2/(C19-F19)</f>
-        <v>1.93034892076503</v>
-      </c>
-      <c r="J19" s="1" t="n">
+      <c r="I19" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,7 +1026,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.6135</v>
@@ -1063,12 +1043,11 @@
       <c r="G20" s="1" t="n">
         <v>3013</v>
       </c>
-      <c r="I20" s="2" t="n">
-        <f aca="false">C20*$K$2/(C20-F20)</f>
-        <v>2.00193258096173</v>
-      </c>
-      <c r="J20" s="1" t="n">
+      <c r="I20" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,9 +1055,9 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="C21" s="4" t="n">
         <v>0.631</v>
       </c>
       <c r="D21" s="1" t="n">
@@ -1093,12 +1072,11 @@
       <c r="G21" s="1" t="n">
         <v>3014</v>
       </c>
-      <c r="I21" s="2" t="n">
-        <f aca="false">C21*$K$2/(C21-F21)</f>
-        <v>1.98313717706364</v>
-      </c>
-      <c r="J21" s="1" t="n">
+      <c r="I21" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,7 +1084,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0.5587</v>
@@ -1117,18 +1095,17 @@
       <c r="E22" s="1" t="n">
         <v>0.3235</v>
       </c>
-      <c r="F22" s="6" t="n">
+      <c r="F22" s="4" t="n">
         <v>0.272</v>
       </c>
       <c r="G22" s="1" t="n">
         <v>3015</v>
       </c>
-      <c r="I22" s="2" t="n">
-        <f aca="false">C22*$K$2/(C22-F22)</f>
-        <v>1.94393302406697</v>
-      </c>
-      <c r="J22" s="1" t="n">
+      <c r="I22" s="1" t="n">
         <v>77</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,7 +1113,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>0.5033</v>
@@ -1154,14 +1131,13 @@
         <v>3016</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" s="2" t="n">
-        <f aca="false">C23*$K$2/(C23-F23)</f>
-        <v>1.9750664122738</v>
-      </c>
-      <c r="J23" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="I23" s="1" t="n">
         <v>77</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1169,7 +1145,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>0.5366</v>
@@ -1187,14 +1163,13 @@
         <v>3017</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I24" s="2" t="n">
-        <f aca="false">C24*$K$2/(C24-F24)</f>
-        <v>1.97666161004431</v>
-      </c>
-      <c r="J24" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="I24" s="1" t="n">
         <v>90</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,7 +1177,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>0.5163</v>
@@ -1219,12 +1194,11 @@
       <c r="G25" s="1" t="n">
         <v>3018</v>
       </c>
-      <c r="I25" s="2" t="n">
-        <f aca="false">C25*$K$2/(C25-F25)</f>
-        <v>1.95161008715423</v>
-      </c>
-      <c r="J25" s="1" t="n">
+      <c r="I25" s="1" t="n">
         <v>90</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,7 +1206,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>0.4602</v>
@@ -1247,14 +1221,13 @@
         <v>0.2125</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" s="2" t="n">
-        <f aca="false">C26*$K$2/(C26-F26)</f>
-        <v>1.85332219620509</v>
-      </c>
-      <c r="J26" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="I26" s="1" t="n">
         <v>80</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,7 +1235,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>0.5738</v>
@@ -1279,12 +1252,11 @@
       <c r="G27" s="1" t="n">
         <v>3019</v>
       </c>
-      <c r="I27" s="2" t="n">
-        <f aca="false">C27*$K$2/(C27-F27)</f>
-        <v>1.90859770590197</v>
-      </c>
-      <c r="J27" s="1" t="n">
+      <c r="I27" s="1" t="n">
         <v>80</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,9 +1264,9 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="6" t="n">
+        <v>41</v>
+      </c>
+      <c r="C28" s="4" t="n">
         <v>0.597</v>
       </c>
       <c r="D28" s="1" t="n">
@@ -1309,12 +1281,11 @@
       <c r="G28" s="1" t="n">
         <v>3020</v>
       </c>
-      <c r="I28" s="2" t="n">
-        <f aca="false">C28*$K$2/(C28-F28)</f>
-        <v>1.97785247426104</v>
-      </c>
-      <c r="J28" s="1" t="n">
+      <c r="I28" s="1" t="n">
         <v>89</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1322,7 +1293,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>0.5927</v>
@@ -1339,12 +1310,11 @@
       <c r="G29" s="1" t="n">
         <v>3021</v>
       </c>
-      <c r="I29" s="2" t="n">
-        <f aca="false">C29*$K$2/(C29-F29)</f>
-        <v>1.99138416301785</v>
-      </c>
-      <c r="J29" s="1" t="n">
+      <c r="I29" s="1" t="n">
         <v>89</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1352,7 +1322,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>0.6155</v>
@@ -1369,12 +1339,11 @@
       <c r="G30" s="1" t="n">
         <v>3022</v>
       </c>
-      <c r="I30" s="2" t="n">
-        <f aca="false">C30*$K$2/(C30-F30)</f>
-        <v>2.00911606675393</v>
-      </c>
-      <c r="J30" s="1" t="n">
+      <c r="I30" s="1" t="n">
         <v>89</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,7 +1351,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>0.5128</v>
@@ -1393,18 +1362,17 @@
       <c r="E31" s="1" t="n">
         <v>0.2987</v>
       </c>
-      <c r="F31" s="6" t="n">
+      <c r="F31" s="4" t="n">
         <v>0.251</v>
       </c>
       <c r="G31" s="1" t="n">
         <v>3023</v>
       </c>
-      <c r="I31" s="2" t="n">
-        <f aca="false">C31*$K$2/(C31-F31)</f>
-        <v>1.95392861726509</v>
-      </c>
-      <c r="J31" s="1" t="n">
+      <c r="I31" s="1" t="n">
         <v>89</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1412,7 +1380,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>0.6009</v>
@@ -1429,12 +1397,11 @@
       <c r="G32" s="1" t="n">
         <v>3024</v>
       </c>
-      <c r="I32" s="2" t="n">
-        <f aca="false">C32*$K$2/(C32-F32)</f>
-        <v>1.97503059637562</v>
-      </c>
-      <c r="J32" s="1" t="n">
+      <c r="I32" s="1" t="n">
         <v>78</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,9 +1409,9 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="6" t="n">
+        <v>46</v>
+      </c>
+      <c r="C33" s="4" t="n">
         <v>0.537</v>
       </c>
       <c r="D33" s="1" t="n">
@@ -1459,12 +1426,11 @@
       <c r="G33" s="1" t="n">
         <v>3025</v>
       </c>
-      <c r="I33" s="2" t="n">
-        <f aca="false">C33*$K$2/(C33-F33)</f>
-        <v>1.97813508124077</v>
-      </c>
-      <c r="J33" s="1" t="n">
+      <c r="I33" s="1" t="n">
         <v>79</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1472,7 +1438,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>0.5782</v>
@@ -1489,12 +1455,11 @@
       <c r="G34" s="1" t="n">
         <v>3026</v>
       </c>
-      <c r="I34" s="2" t="n">
-        <f aca="false">C34*$K$2/(C34-F34)</f>
-        <v>1.95584139708376</v>
-      </c>
-      <c r="J34" s="1" t="n">
+      <c r="I34" s="1" t="n">
         <v>96</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1502,7 +1467,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>0.5304</v>
@@ -1519,12 +1484,11 @@
       <c r="G35" s="1" t="n">
         <v>3027</v>
       </c>
-      <c r="I35" s="2" t="n">
-        <f aca="false">C35*$K$2/(C35-F35)</f>
-        <v>1.90185196261682</v>
-      </c>
-      <c r="J35" s="1" t="n">
+      <c r="I35" s="1" t="n">
         <v>74</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,7 +1496,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>0.4571</v>
@@ -1549,12 +1513,11 @@
       <c r="G36" s="1" t="n">
         <v>3028</v>
       </c>
-      <c r="I36" s="2" t="n">
-        <f aca="false">C36*$K$2/(C36-F36)</f>
-        <v>1.94197416524702</v>
-      </c>
-      <c r="J36" s="1" t="n">
+      <c r="I36" s="1" t="n">
         <v>74</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,9 +1525,9 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="C37" s="4" t="n">
         <v>0.384</v>
       </c>
       <c r="D37" s="1" t="n">
@@ -1579,12 +1542,11 @@
       <c r="G37" s="1" t="n">
         <v>3029</v>
       </c>
-      <c r="I37" s="2" t="n">
-        <f aca="false">C37*$K$2/(C37-F37)</f>
-        <v>1.81974042755344</v>
-      </c>
-      <c r="J37" s="1" t="n">
+      <c r="I37" s="1" t="n">
         <v>92</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1592,7 +1554,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>0.5799</v>
@@ -1609,12 +1571,11 @@
       <c r="G38" s="1" t="n">
         <v>3030</v>
       </c>
-      <c r="I38" s="2" t="n">
-        <f aca="false">C38*$K$2/(C38-F38)</f>
-        <v>1.99611265010352</v>
-      </c>
-      <c r="J38" s="1" t="n">
+      <c r="I38" s="1" t="n">
         <v>65</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,7 +1583,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>0.5348</v>
@@ -1640,14 +1601,13 @@
         <v>3031</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I39" s="2" t="n">
-        <f aca="false">C39*$K$2/(C39-F39)</f>
-        <v>1.99508</v>
-      </c>
-      <c r="J39" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="I39" s="1" t="n">
         <v>88</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,7 +1615,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>0.6018</v>
@@ -1672,12 +1632,11 @@
       <c r="G40" s="1" t="n">
         <v>3032</v>
       </c>
-      <c r="I40" s="2" t="n">
-        <f aca="false">C40*$K$2/(C40-F40)</f>
-        <v>1.97278860335196</v>
-      </c>
-      <c r="J40" s="1" t="n">
+      <c r="I40" s="1" t="n">
         <v>88</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,9 +1644,9 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="C41" s="4" t="n">
         <v>0.52</v>
       </c>
       <c r="D41" s="1" t="n">
@@ -1702,17 +1661,14 @@
       <c r="G41" s="1" t="n">
         <v>3033</v>
       </c>
-      <c r="I41" s="2" t="n">
-        <f aca="false">C41*$K$2/(C41-F41)</f>
-        <v>1.91268731563422</v>
-      </c>
+      <c r="J41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>0.5154</v>
@@ -1723,16 +1679,58 @@
       <c r="G42" s="1" t="n">
         <v>3112</v>
       </c>
-      <c r="J42" s="1" t="n">
+      <c r="I42" s="1" t="n">
         <v>76</v>
       </c>
+      <c r="J42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1"/>
+      <c r="AB42" s="1"/>
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1"/>
+      <c r="AE42" s="1"/>
+      <c r="AF42" s="1"/>
+      <c r="AG42" s="1"/>
+      <c r="AH42" s="1"/>
+      <c r="AI42" s="1"/>
+      <c r="AJ42" s="1"/>
+      <c r="AK42" s="1"/>
+      <c r="AL42" s="1"/>
+      <c r="AM42" s="1"/>
+      <c r="AN42" s="1"/>
+      <c r="AO42" s="1"/>
+      <c r="AP42" s="1"/>
+      <c r="AQ42" s="1"/>
+      <c r="AR42" s="1"/>
+      <c r="AS42" s="1"/>
+      <c r="AT42" s="1"/>
+      <c r="AU42" s="1"/>
+      <c r="AV42" s="1"/>
+      <c r="AW42" s="1"/>
+      <c r="AX42" s="1"/>
+      <c r="AY42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>0.5808</v>
@@ -1743,8 +1741,11 @@
       <c r="G43" s="1" t="n">
         <v>3105</v>
       </c>
-      <c r="J43" s="1" t="n">
+      <c r="I43" s="1" t="n">
         <v>81</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1752,7 +1753,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>0.5297</v>
@@ -1763,8 +1764,11 @@
       <c r="G44" s="1" t="n">
         <v>3106</v>
       </c>
-      <c r="J44" s="1" t="n">
+      <c r="I44" s="1" t="n">
         <v>96</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,7 +1776,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>0.6231</v>
@@ -1783,8 +1787,11 @@
       <c r="G45" s="1" t="n">
         <v>3107</v>
       </c>
-      <c r="J45" s="1" t="n">
+      <c r="I45" s="1" t="n">
         <v>77</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1792,7 +1799,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>0.5526</v>
@@ -1803,8 +1810,11 @@
       <c r="G46" s="1" t="n">
         <v>3108</v>
       </c>
-      <c r="J46" s="1" t="n">
+      <c r="I46" s="1" t="n">
         <v>77</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,7 +1822,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>0.6166</v>
@@ -1823,8 +1833,11 @@
       <c r="G47" s="1" t="n">
         <v>3109</v>
       </c>
-      <c r="J47" s="1" t="n">
+      <c r="I47" s="1" t="n">
         <v>79</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1832,7 +1845,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>0.616</v>
@@ -1843,8 +1856,14 @@
       <c r="G48" s="1" t="n">
         <v>3110</v>
       </c>
-      <c r="J48" s="1" t="n">
+      <c r="H48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I48" s="1" t="n">
         <v>79</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,7 +1871,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>0.6012</v>
@@ -1863,8 +1882,11 @@
       <c r="G49" s="1" t="n">
         <v>3111</v>
       </c>
-      <c r="J49" s="1" t="n">
+      <c r="I49" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,7 +1894,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>0.6259</v>
@@ -1883,8 +1905,11 @@
       <c r="G50" s="1" t="n">
         <v>3102</v>
       </c>
-      <c r="J50" s="1" t="n">
+      <c r="I50" s="1" t="n">
         <v>75</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,7 +1917,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>0.4081</v>
@@ -1903,8 +1928,11 @@
       <c r="G51" s="1" t="n">
         <v>3103</v>
       </c>
-      <c r="J51" s="1" t="n">
+      <c r="I51" s="1" t="n">
         <v>75</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1912,7 +1940,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>0.6034</v>
@@ -1923,8 +1951,11 @@
       <c r="G52" s="1" t="n">
         <v>3104</v>
       </c>
-      <c r="J52" s="1" t="n">
+      <c r="I52" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1932,7 +1963,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>0.558</v>
@@ -1943,8 +1974,11 @@
       <c r="G53" s="1" t="n">
         <v>3095</v>
       </c>
-      <c r="J53" s="1" t="n">
+      <c r="I53" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,7 +1986,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>0.5753</v>
@@ -1963,8 +1997,11 @@
       <c r="G54" s="1" t="n">
         <v>3096</v>
       </c>
-      <c r="J54" s="1" t="n">
+      <c r="I54" s="1" t="n">
         <v>79</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,7 +2009,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>0.5093</v>
@@ -1983,8 +2020,11 @@
       <c r="G55" s="1" t="n">
         <v>3097</v>
       </c>
-      <c r="J55" s="1" t="n">
+      <c r="I55" s="1" t="n">
         <v>79</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,7 +2032,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>0.543</v>
@@ -2003,8 +2043,11 @@
       <c r="G56" s="1" t="n">
         <v>3098</v>
       </c>
-      <c r="J56" s="1" t="n">
+      <c r="I56" s="1" t="n">
         <v>84</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,7 +2055,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>0.6157</v>
@@ -2023,8 +2066,11 @@
       <c r="G57" s="1" t="n">
         <v>3099</v>
       </c>
-      <c r="J57" s="1" t="n">
+      <c r="I57" s="1" t="n">
         <v>84</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,7 +2078,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>0.5963</v>
@@ -2043,8 +2089,11 @@
       <c r="G58" s="1" t="n">
         <v>3100</v>
       </c>
-      <c r="J58" s="1" t="n">
+      <c r="I58" s="1" t="n">
         <v>78</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,7 +2101,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>0.6115</v>
@@ -2063,8 +2112,14 @@
       <c r="G59" s="1" t="n">
         <v>3101</v>
       </c>
-      <c r="J59" s="1" t="n">
+      <c r="H59" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I59" s="1" t="n">
         <v>78</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2072,7 +2127,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>0.62</v>
@@ -2083,8 +2138,11 @@
       <c r="G60" s="1" t="n">
         <v>3093</v>
       </c>
-      <c r="J60" s="1" t="n">
+      <c r="I60" s="1" t="n">
         <v>78</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2092,7 +2150,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>0.5576</v>
@@ -2103,8 +2161,11 @@
       <c r="G61" s="1" t="n">
         <v>3094</v>
       </c>
-      <c r="J61" s="1" t="n">
+      <c r="I61" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2112,7 +2173,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>0.5735</v>
@@ -2123,8 +2184,11 @@
       <c r="G62" s="1" t="n">
         <v>3092</v>
       </c>
-      <c r="J62" s="1" t="n">
+      <c r="I62" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2132,7 +2196,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>0.6063</v>
@@ -2143,8 +2207,11 @@
       <c r="G63" s="1" t="n">
         <v>3088</v>
       </c>
-      <c r="J63" s="1" t="n">
+      <c r="I63" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2219,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>0.5711</v>
@@ -2163,8 +2230,11 @@
       <c r="G64" s="1" t="n">
         <v>3089</v>
       </c>
-      <c r="J64" s="1" t="n">
+      <c r="I64" s="1" t="n">
         <v>92</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2172,7 +2242,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>0.5817</v>
@@ -2183,8 +2253,11 @@
       <c r="G65" s="1" t="n">
         <v>3090</v>
       </c>
-      <c r="J65" s="1" t="n">
+      <c r="I65" s="1" t="n">
         <v>92</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,7 +2265,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>0.5617</v>
@@ -2203,8 +2276,11 @@
       <c r="G66" s="1" t="n">
         <v>3091</v>
       </c>
-      <c r="J66" s="1" t="n">
+      <c r="I66" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,7 +2288,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>0.5667</v>
@@ -2223,8 +2299,11 @@
       <c r="G67" s="1" t="n">
         <v>3081</v>
       </c>
-      <c r="J67" s="1" t="n">
+      <c r="I67" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,7 +2311,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>0.5488</v>
@@ -2243,8 +2322,11 @@
       <c r="G68" s="1" t="n">
         <v>3082</v>
       </c>
-      <c r="J68" s="1" t="n">
+      <c r="I68" s="1" t="n">
         <v>79</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2252,7 +2334,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>0.5118</v>
@@ -2263,8 +2345,11 @@
       <c r="G69" s="1" t="n">
         <v>3083</v>
       </c>
-      <c r="J69" s="1" t="n">
+      <c r="I69" s="1" t="n">
         <v>96</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2272,7 +2357,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>0.4949</v>
@@ -2286,8 +2371,11 @@
       <c r="G70" s="1" t="n">
         <v>3084</v>
       </c>
-      <c r="J70" s="1" t="n">
+      <c r="I70" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,7 +2383,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>0.5966</v>
@@ -2309,8 +2397,11 @@
       <c r="G71" s="1" t="n">
         <v>3085</v>
       </c>
-      <c r="J71" s="1" t="n">
+      <c r="I71" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,7 +2409,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>0.5994</v>
@@ -2332,8 +2423,11 @@
       <c r="G72" s="1" t="n">
         <v>3074</v>
       </c>
-      <c r="J72" s="1" t="n">
+      <c r="I72" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,7 +2435,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>0.5666</v>
@@ -2355,8 +2449,11 @@
       <c r="G73" s="1" t="n">
         <v>3075</v>
       </c>
-      <c r="J73" s="1" t="n">
+      <c r="I73" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,7 +2461,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>0.5385</v>
@@ -2378,8 +2475,11 @@
       <c r="G74" s="1" t="n">
         <v>3076</v>
       </c>
-      <c r="J74" s="1" t="n">
+      <c r="I74" s="1" t="n">
         <v>89</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2387,7 +2487,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>0.5566</v>
@@ -2401,8 +2501,11 @@
       <c r="G75" s="1" t="n">
         <v>3079</v>
       </c>
-      <c r="J75" s="1" t="n">
+      <c r="I75" s="1" t="n">
         <v>74</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,7 +2513,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>0.5749</v>
@@ -2424,8 +2527,11 @@
       <c r="G76" s="1" t="n">
         <v>3080</v>
       </c>
-      <c r="J76" s="1" t="n">
+      <c r="I76" s="1" t="n">
         <v>82</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2433,7 +2539,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>0.5927</v>
@@ -2447,8 +2553,11 @@
       <c r="G77" s="1" t="n">
         <v>3071</v>
       </c>
-      <c r="J77" s="1" t="n">
+      <c r="I77" s="1" t="n">
         <v>82</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2456,7 +2565,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>0.5992</v>
@@ -2470,8 +2579,11 @@
       <c r="G78" s="1" t="n">
         <v>3072</v>
       </c>
-      <c r="J78" s="1" t="n">
+      <c r="I78" s="1" t="n">
         <v>69</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2479,7 +2591,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>0.5788</v>
@@ -2493,8 +2605,11 @@
       <c r="G79" s="1" t="n">
         <v>3073</v>
       </c>
-      <c r="J79" s="1" t="n">
+      <c r="I79" s="1" t="n">
         <v>69</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,7 +2617,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>0.5113</v>
@@ -2516,8 +2631,11 @@
       <c r="G80" s="1" t="n">
         <v>3077</v>
       </c>
-      <c r="J80" s="1" t="n">
+      <c r="I80" s="1" t="n">
         <v>75</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,7 +2643,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>0.577</v>
@@ -2539,14 +2657,17 @@
       <c r="G81" s="1" t="n">
         <v>3078</v>
       </c>
-      <c r="J81" s="1" t="n">
+      <c r="I81" s="1" t="n">
         <v>78</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
adapted to full sample set
</commit_message>
<xml_diff>
--- a/02_Data/03_Scale/Gravimetric_analysis.xlsx
+++ b/02_Data/03_Scale/Gravimetric_analysis.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="98">
   <si>
     <t xml:space="preserve">Sample Nr</t>
   </si>
@@ -55,13 +55,22 @@
     <t xml:space="preserve">sex</t>
   </si>
   <si>
+    <t xml:space="preserve">site</t>
+  </si>
+  <si>
     <t xml:space="preserve">385_L</t>
   </si>
   <si>
     <t xml:space="preserve">F</t>
   </si>
   <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
     <t xml:space="preserve">385_R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
   </si>
   <si>
     <t xml:space="preserve">386_L</t>
@@ -445,7 +454,7 @@
   <dimension ref="A1:AY81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -496,13 +505,16 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0.5551</v>
@@ -523,9 +535,11 @@
         <v>87</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="M2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0.5426</v>
@@ -554,7 +568,10 @@
         <v>87</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,7 +579,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0.6119</v>
@@ -583,7 +600,10 @@
         <v>76</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,7 +611,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0.5484</v>
@@ -612,7 +632,10 @@
         <v>81</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,7 +643,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0.5622</v>
@@ -641,7 +664,10 @@
         <v>88</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,7 +675,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0.5647</v>
@@ -670,7 +696,10 @@
         <v>88</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.5565</v>
@@ -699,7 +728,10 @@
         <v>91</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,7 +739,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0.5834</v>
@@ -728,7 +760,10 @@
         <v>91</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,7 +771,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0.4961</v>
@@ -751,13 +786,16 @@
         <v>0.2127</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>96</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,7 +803,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0.5625</v>
@@ -786,7 +824,10 @@
         <v>94</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,7 +835,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0.5694</v>
@@ -815,7 +856,10 @@
         <v>94</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,7 +867,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.5793</v>
@@ -844,7 +888,10 @@
         <v>78</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,7 +899,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>0.538</v>
@@ -873,7 +920,10 @@
         <v>78</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -881,7 +931,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0.5547</v>
@@ -902,7 +952,10 @@
         <v>91</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,7 +963,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.4772</v>
@@ -925,13 +978,16 @@
         <v>0.2224</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I16" s="1" t="n">
         <v>91</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,7 +995,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.5973</v>
@@ -960,7 +1016,10 @@
         <v>64</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,7 +1027,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0.6042</v>
@@ -989,7 +1048,10 @@
         <v>64</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,7 +1059,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0.5666</v>
@@ -1018,7 +1080,10 @@
         <v>71</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,7 +1091,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.6135</v>
@@ -1047,7 +1112,10 @@
         <v>85</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,7 +1123,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>0.631</v>
@@ -1076,7 +1144,10 @@
         <v>85</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,7 +1155,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0.5587</v>
@@ -1105,7 +1176,10 @@
         <v>77</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,7 +1187,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>0.5033</v>
@@ -1131,13 +1205,16 @@
         <v>3016</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I23" s="1" t="n">
         <v>77</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,7 +1222,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>0.5366</v>
@@ -1163,13 +1240,16 @@
         <v>3017</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I24" s="1" t="n">
         <v>90</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,7 +1257,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>0.5163</v>
@@ -1198,7 +1278,10 @@
         <v>90</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,7 +1289,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>0.4602</v>
@@ -1221,13 +1304,16 @@
         <v>0.2125</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I26" s="1" t="n">
         <v>80</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1235,7 +1321,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>0.5738</v>
@@ -1256,7 +1342,10 @@
         <v>80</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,7 +1353,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>0.597</v>
@@ -1285,7 +1374,10 @@
         <v>89</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,7 +1385,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>0.5927</v>
@@ -1314,7 +1406,10 @@
         <v>89</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1322,7 +1417,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>0.6155</v>
@@ -1343,7 +1438,10 @@
         <v>89</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1351,7 +1449,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>0.5128</v>
@@ -1372,7 +1470,10 @@
         <v>89</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,7 +1481,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>0.6009</v>
@@ -1401,7 +1502,10 @@
         <v>78</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1409,7 +1513,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>0.537</v>
@@ -1430,7 +1534,10 @@
         <v>79</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1438,7 +1545,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>0.5782</v>
@@ -1459,7 +1566,10 @@
         <v>96</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,7 +1577,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>0.5304</v>
@@ -1488,7 +1598,10 @@
         <v>74</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,7 +1609,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>0.4571</v>
@@ -1517,7 +1630,10 @@
         <v>74</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1525,7 +1641,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C37" s="4" t="n">
         <v>0.384</v>
@@ -1546,7 +1662,10 @@
         <v>92</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,7 +1673,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>0.5799</v>
@@ -1575,7 +1694,10 @@
         <v>65</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1583,7 +1705,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>0.5348</v>
@@ -1601,13 +1723,16 @@
         <v>3031</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I39" s="1" t="n">
         <v>88</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1615,7 +1740,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>0.6018</v>
@@ -1636,7 +1761,10 @@
         <v>88</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,7 +1772,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>0.52</v>
@@ -1662,13 +1790,16 @@
         <v>3033</v>
       </c>
       <c r="J41" s="4"/>
+      <c r="K41" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>0.5154</v>
@@ -1683,7 +1814,10 @@
         <v>76</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
@@ -1730,7 +1864,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>0.5808</v>
@@ -1745,7 +1879,10 @@
         <v>81</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,7 +1890,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>0.5297</v>
@@ -1768,7 +1905,10 @@
         <v>96</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,7 +1916,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>0.6231</v>
@@ -1791,7 +1931,10 @@
         <v>77</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,7 +1942,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>0.5526</v>
@@ -1814,7 +1957,10 @@
         <v>77</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,7 +1968,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>0.6166</v>
@@ -1837,7 +1983,10 @@
         <v>79</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,7 +1994,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>0.616</v>
@@ -1857,13 +2006,16 @@
         <v>3110</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I48" s="1" t="n">
         <v>79</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,7 +2023,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>0.6012</v>
@@ -1886,7 +2038,10 @@
         <v>71</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +2049,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>0.6259</v>
@@ -1909,7 +2064,10 @@
         <v>75</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,7 +2075,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>0.4081</v>
@@ -1932,7 +2090,10 @@
         <v>75</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,7 +2101,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>0.6034</v>
@@ -1955,7 +2116,10 @@
         <v>60</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,7 +2127,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>0.558</v>
@@ -1978,7 +2142,10 @@
         <v>60</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1986,7 +2153,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>0.5753</v>
@@ -2001,7 +2168,10 @@
         <v>79</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,7 +2179,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>0.5093</v>
@@ -2024,7 +2194,10 @@
         <v>79</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,7 +2205,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>0.543</v>
@@ -2047,7 +2220,10 @@
         <v>84</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,7 +2231,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>0.6157</v>
@@ -2070,7 +2246,10 @@
         <v>84</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2078,7 +2257,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>0.5963</v>
@@ -2093,7 +2272,10 @@
         <v>78</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,7 +2283,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>0.6115</v>
@@ -2113,13 +2295,16 @@
         <v>3101</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I59" s="1" t="n">
         <v>78</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2127,7 +2312,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>0.62</v>
@@ -2142,7 +2327,10 @@
         <v>78</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2150,7 +2338,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>0.5576</v>
@@ -2165,7 +2353,10 @@
         <v>57</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,7 +2364,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>0.5735</v>
@@ -2188,7 +2379,10 @@
         <v>85</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2390,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>0.6063</v>
@@ -2211,7 +2405,10 @@
         <v>85</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2219,7 +2416,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>0.5711</v>
@@ -2234,7 +2431,10 @@
         <v>92</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,7 +2442,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>0.5817</v>
@@ -2257,7 +2457,10 @@
         <v>92</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2265,7 +2468,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>0.5617</v>
@@ -2280,7 +2483,10 @@
         <v>85</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2288,7 +2494,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>0.5667</v>
@@ -2303,7 +2509,10 @@
         <v>85</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,7 +2520,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>0.5488</v>
@@ -2326,7 +2535,10 @@
         <v>79</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2334,7 +2546,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>0.5118</v>
@@ -2349,7 +2561,10 @@
         <v>96</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2357,7 +2572,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>0.4949</v>
@@ -2375,7 +2590,10 @@
         <v>71</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2383,7 +2601,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>0.5966</v>
@@ -2401,7 +2619,10 @@
         <v>71</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2409,7 +2630,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>0.5994</v>
@@ -2427,7 +2648,10 @@
         <v>85</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2435,7 +2659,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>0.5666</v>
@@ -2453,7 +2677,10 @@
         <v>85</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2461,7 +2688,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>0.5385</v>
@@ -2479,7 +2706,10 @@
         <v>89</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2487,7 +2717,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>0.5566</v>
@@ -2505,7 +2735,10 @@
         <v>74</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2513,7 +2746,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>0.5749</v>
@@ -2531,7 +2764,10 @@
         <v>82</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,7 +2775,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>0.5927</v>
@@ -2557,7 +2793,10 @@
         <v>82</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,7 +2804,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>0.5992</v>
@@ -2583,7 +2822,10 @@
         <v>69</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2591,7 +2833,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>0.5788</v>
@@ -2609,7 +2851,10 @@
         <v>69</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2617,7 +2862,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>0.5113</v>
@@ -2635,7 +2880,10 @@
         <v>75</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2643,7 +2891,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>0.577</v>
@@ -2661,7 +2909,10 @@
         <v>78</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajusted failure data (removal of measurement errors at end of curve)
</commit_message>
<xml_diff>
--- a/02_Data/03_Scale/Gravimetric_analysis.xlsx
+++ b/02_Data/03_Scale/Gravimetric_analysis.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="99">
   <si>
     <t xml:space="preserve">Sample Nr</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t xml:space="preserve">422_R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tracking issue</t>
   </si>
   <si>
     <t xml:space="preserve">423_R</t>
@@ -454,7 +457,7 @@
   <dimension ref="A1:AY81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E70" activeCellId="0" sqref="E70"/>
+      <selection pane="topLeft" activeCell="H48" activeCellId="0" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2437,6 +2440,9 @@
       <c r="G60" s="1" t="n">
         <v>3093</v>
       </c>
+      <c r="H60" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I60" s="1" t="n">
         <v>78</v>
       </c>
@@ -2748,6 +2754,9 @@
       <c r="D70" s="1" t="n">
         <v>0.472</v>
       </c>
+      <c r="E70" s="1" t="n">
+        <v>0.3028</v>
+      </c>
       <c r="F70" s="1" t="n">
         <v>0.2537</v>
       </c>
@@ -2777,6 +2786,9 @@
       <c r="D71" s="1" t="n">
         <v>0.5683</v>
       </c>
+      <c r="E71" s="1" t="n">
+        <v>0.3653</v>
+      </c>
       <c r="F71" s="1" t="n">
         <v>0.3057</v>
       </c>
@@ -2806,6 +2818,9 @@
       <c r="D72" s="1" t="n">
         <v>0.571</v>
       </c>
+      <c r="E72" s="1" t="n">
+        <v>0.3626</v>
+      </c>
       <c r="F72" s="1" t="n">
         <v>0.3024</v>
       </c>
@@ -2835,11 +2850,17 @@
       <c r="D73" s="1" t="n">
         <v>0.5414</v>
       </c>
+      <c r="E73" s="1" t="n">
+        <v>0.3379</v>
+      </c>
       <c r="F73" s="1" t="n">
         <v>0.2815</v>
       </c>
       <c r="G73" s="1" t="n">
         <v>3075</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="I73" s="1" t="n">
         <v>85</v>
@@ -2856,13 +2877,16 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>0.5385</v>
       </c>
       <c r="D74" s="1" t="n">
         <v>0.5115</v>
+      </c>
+      <c r="E74" s="1" t="n">
+        <v>0.3227</v>
       </c>
       <c r="F74" s="1" t="n">
         <v>0.27</v>
@@ -2885,13 +2909,16 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>0.5566</v>
       </c>
       <c r="D75" s="1" t="n">
         <v>0.5293</v>
+      </c>
+      <c r="E75" s="1" t="n">
+        <v>0.3292</v>
       </c>
       <c r="F75" s="1" t="n">
         <v>0.2788</v>
@@ -2914,13 +2941,16 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>0.5749</v>
       </c>
       <c r="D76" s="1" t="n">
         <v>0.5444</v>
+      </c>
+      <c r="E76" s="1" t="n">
+        <v>0.3376</v>
       </c>
       <c r="F76" s="1" t="n">
         <v>0.2828</v>
@@ -2943,13 +2973,16 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>0.5927</v>
       </c>
       <c r="D77" s="1" t="n">
         <v>0.5678</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>0.3605</v>
       </c>
       <c r="F77" s="1" t="n">
         <v>0.3035</v>
@@ -2972,7 +3005,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>0.5992</v>
@@ -2980,11 +3013,17 @@
       <c r="D78" s="1" t="n">
         <v>0.5699</v>
       </c>
+      <c r="E78" s="1" t="n">
+        <v>0.3577</v>
+      </c>
       <c r="F78" s="1" t="n">
         <v>0.3003</v>
       </c>
       <c r="G78" s="1" t="n">
         <v>3072</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="I78" s="1" t="n">
         <v>69</v>
@@ -3001,13 +3040,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>0.5788</v>
       </c>
       <c r="D79" s="1" t="n">
         <v>0.5522</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>0.3489</v>
       </c>
       <c r="F79" s="1" t="n">
         <v>0.2899</v>
@@ -3030,13 +3072,16 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>0.5113</v>
       </c>
       <c r="D80" s="1" t="n">
         <v>0.4856</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>0.3094</v>
       </c>
       <c r="F80" s="1" t="n">
         <v>0.2593</v>
@@ -3059,13 +3104,16 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>0.577</v>
       </c>
       <c r="D81" s="1" t="n">
         <v>0.5491</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <v>0.34</v>
       </c>
       <c r="F81" s="1" t="n">
         <v>0.2907</v>

</xml_diff>

<commit_message>
update graphs and corresponding scripts to work again
</commit_message>
<xml_diff>
--- a/02_Data/03_Scale/Gravimetric_analysis.xlsx
+++ b/02_Data/03_Scale/Gravimetric_analysis.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$H$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$L$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -31,6 +31,18 @@
     <t xml:space="preserve">Sample ID</t>
   </si>
   <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uCT ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">wet weight</t>
   </si>
   <si>
@@ -43,19 +55,7 @@
     <t xml:space="preserve">H2O weight</t>
   </si>
   <si>
-    <t xml:space="preserve">uCT ID</t>
-  </si>
-  <si>
     <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site</t>
   </si>
   <si>
     <t xml:space="preserve">385_L</t>
@@ -454,27 +454,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AY81"/>
+  <dimension ref="A1:BC81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H48" activeCellId="0" sqref="H48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L36" activeCellId="0" sqref="L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="8.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="13" style="2" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="2" width="10.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,31 +519,31 @@
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>2997</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>0.5551</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="H2" s="1" t="n">
         <v>0.5185</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="I2" s="1" t="n">
         <v>0.3242</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="J2" s="1" t="n">
         <v>0.2657</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <v>2997</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="1"/>
+      <c r="Q2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -553,28 +553,28 @@
         <v>14</v>
       </c>
       <c r="C3" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>2998</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>0.5426</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="H3" s="1" t="n">
         <v>0.5108</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <v>0.3183</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="J3" s="1" t="n">
         <v>0.2638</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>2998</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,28 +585,28 @@
         <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>2999</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>0.6119</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="H4" s="1" t="n">
         <v>0.5777</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="I4" s="1" t="n">
         <v>0.3638</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="J4" s="1" t="n">
         <v>0.3036</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>2999</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,28 +617,28 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>3000</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>0.5484</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="H5" s="1" t="n">
         <v>0.5143</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="I5" s="1" t="n">
         <v>0.319</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="J5" s="1" t="n">
         <v>0.2664</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>3000</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,28 +649,28 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>3001</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <v>0.5622</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="H6" s="1" t="n">
         <v>0.5337</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="I6" s="1" t="n">
         <v>0.3272</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="J6" s="1" t="n">
         <v>0.2785</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>3001</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -681,28 +681,28 @@
         <v>20</v>
       </c>
       <c r="C7" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>3002</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <v>0.5647</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="H7" s="1" t="n">
         <v>0.533</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="I7" s="1" t="n">
         <v>0.3341</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="J7" s="1" t="n">
         <v>0.2811</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>3002</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,28 +713,28 @@
         <v>21</v>
       </c>
       <c r="C8" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>3003</v>
+      </c>
+      <c r="G8" s="1" t="n">
         <v>0.5565</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="H8" s="1" t="n">
         <v>0.5273</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="I8" s="1" t="n">
         <v>0.333</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="J8" s="1" t="n">
         <v>0.2796</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>3003</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,28 +745,28 @@
         <v>22</v>
       </c>
       <c r="C9" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>3004</v>
+      </c>
+      <c r="G9" s="1" t="n">
         <v>0.5834</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="H9" s="1" t="n">
         <v>0.5545</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="I9" s="1" t="n">
         <v>0.3501</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="J9" s="1" t="n">
         <v>0.2926</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>3004</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -777,28 +777,28 @@
         <v>23</v>
       </c>
       <c r="C10" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="n">
         <v>0.4961</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="H10" s="1" t="n">
         <v>0.4404</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="I10" s="1" t="n">
         <v>0.2739</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="J10" s="1" t="n">
         <v>0.2127</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="I10" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -809,28 +809,28 @@
         <v>25</v>
       </c>
       <c r="C11" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>3005</v>
+      </c>
+      <c r="G11" s="1" t="n">
         <v>0.5625</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="H11" s="1" t="n">
         <v>0.5277</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="I11" s="1" t="n">
         <v>0.3279</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="J11" s="1" t="n">
         <v>0.2734</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>3005</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,28 +841,28 @@
         <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>3006</v>
+      </c>
+      <c r="G12" s="1" t="n">
         <v>0.5694</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="H12" s="1" t="n">
         <v>0.5353</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="I12" s="1" t="n">
         <v>0.3346</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="J12" s="1" t="n">
         <v>0.2773</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>3006</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -873,28 +873,28 @@
         <v>27</v>
       </c>
       <c r="C13" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>3007</v>
+      </c>
+      <c r="G13" s="1" t="n">
         <v>0.5793</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="H13" s="1" t="n">
         <v>0.5423</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="I13" s="1" t="n">
         <v>0.3361</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="J13" s="1" t="n">
         <v>0.2804</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>3007</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,29 +904,29 @@
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4" t="n">
+      <c r="C14" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>3008</v>
+      </c>
+      <c r="G14" s="4" t="n">
         <v>0.538</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="H14" s="1" t="n">
         <v>0.5088</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="I14" s="1" t="n">
         <v>0.3187</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="J14" s="1" t="n">
         <v>0.2585</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>3008</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,28 +937,28 @@
         <v>29</v>
       </c>
       <c r="C15" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>3009</v>
+      </c>
+      <c r="G15" s="1" t="n">
         <v>0.5547</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="H15" s="1" t="n">
         <v>0.5133</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="I15" s="1" t="n">
         <v>0.322</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="J15" s="1" t="n">
         <v>0.2663</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>3009</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,28 +969,28 @@
         <v>30</v>
       </c>
       <c r="C16" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="1" t="n">
         <v>0.4772</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="H16" s="1" t="n">
         <v>0.4484</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="I16" s="1" t="n">
         <v>0.2795</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="J16" s="1" t="n">
         <v>0.2224</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,28 +1001,28 @@
         <v>31</v>
       </c>
       <c r="C17" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>3010</v>
+      </c>
+      <c r="G17" s="1" t="n">
         <v>0.5973</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="H17" s="1" t="n">
         <v>0.5683</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="I17" s="1" t="n">
         <v>0.3543</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="J17" s="1" t="n">
         <v>0.2991</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>3010</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,28 +1033,28 @@
         <v>32</v>
       </c>
       <c r="C18" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>3011</v>
+      </c>
+      <c r="G18" s="1" t="n">
         <v>0.6042</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="H18" s="1" t="n">
         <v>0.5724</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="I18" s="1" t="n">
         <v>0.3602</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="J18" s="1" t="n">
         <v>0.3012</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>3011</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,28 +1065,28 @@
         <v>33</v>
       </c>
       <c r="C19" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>3012</v>
+      </c>
+      <c r="G19" s="1" t="n">
         <v>0.5666</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="H19" s="1" t="n">
         <v>0.5337</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="I19" s="1" t="n">
         <v>0.3299</v>
       </c>
-      <c r="F19" s="1" t="n">
+      <c r="J19" s="1" t="n">
         <v>0.2738</v>
-      </c>
-      <c r="G19" s="1" t="n">
-        <v>3012</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,28 +1097,28 @@
         <v>34</v>
       </c>
       <c r="C20" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>3013</v>
+      </c>
+      <c r="G20" s="1" t="n">
         <v>0.6135</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="H20" s="1" t="n">
         <v>0.5848</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="I20" s="1" t="n">
         <v>0.368</v>
       </c>
-      <c r="F20" s="1" t="n">
+      <c r="J20" s="1" t="n">
         <v>0.3078</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>3013</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1128,29 +1128,29 @@
       <c r="B21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="4" t="n">
+      <c r="C21" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>3014</v>
+      </c>
+      <c r="G21" s="4" t="n">
         <v>0.631</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="H21" s="1" t="n">
         <v>0.5986</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="I21" s="1" t="n">
         <v>0.3763</v>
       </c>
-      <c r="F21" s="1" t="n">
+      <c r="J21" s="1" t="n">
         <v>0.3136</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>3014</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,28 +1161,28 @@
         <v>36</v>
       </c>
       <c r="C22" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>3015</v>
+      </c>
+      <c r="G22" s="1" t="n">
         <v>0.5587</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="H22" s="1" t="n">
         <v>0.5232</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="I22" s="1" t="n">
         <v>0.3235</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="J22" s="4" t="n">
         <v>0.272</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>3015</v>
-      </c>
-      <c r="I22" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,31 +1193,31 @@
         <v>37</v>
       </c>
       <c r="C23" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>3016</v>
+      </c>
+      <c r="G23" s="1" t="n">
         <v>0.5033</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="H23" s="1" t="n">
         <v>0.4738</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="I23" s="1" t="n">
         <v>0.2939</v>
       </c>
-      <c r="F23" s="1" t="n">
+      <c r="J23" s="1" t="n">
         <v>0.2491</v>
       </c>
-      <c r="G23" s="1" t="n">
-        <v>3016</v>
-      </c>
-      <c r="H23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1228,31 +1228,31 @@
         <v>39</v>
       </c>
       <c r="C24" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>3017</v>
+      </c>
+      <c r="G24" s="1" t="n">
         <v>0.5366</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="H24" s="1" t="n">
         <v>0.5039</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="I24" s="1" t="n">
         <v>0.3157</v>
       </c>
-      <c r="F24" s="1" t="n">
+      <c r="J24" s="1" t="n">
         <v>0.2658</v>
       </c>
-      <c r="G24" s="1" t="n">
-        <v>3017</v>
-      </c>
-      <c r="H24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,28 +1263,28 @@
         <v>41</v>
       </c>
       <c r="C25" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>3018</v>
+      </c>
+      <c r="G25" s="1" t="n">
         <v>0.5163</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="H25" s="1" t="n">
         <v>0.4799</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="I25" s="1" t="n">
         <v>0.2977</v>
       </c>
-      <c r="F25" s="1" t="n">
+      <c r="J25" s="1" t="n">
         <v>0.2524</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>3018</v>
-      </c>
-      <c r="I25" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1295,28 +1295,28 @@
         <v>42</v>
       </c>
       <c r="C26" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="1" t="n">
         <v>0.4602</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="H26" s="1" t="n">
         <v>0.4217</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="I26" s="1" t="n">
         <v>0.2646</v>
       </c>
-      <c r="F26" s="1" t="n">
+      <c r="J26" s="1" t="n">
         <v>0.2125</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="I26" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,28 +1327,28 @@
         <v>43</v>
       </c>
       <c r="C27" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>3019</v>
+      </c>
+      <c r="G27" s="1" t="n">
         <v>0.5738</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="H27" s="1" t="n">
         <v>0.5241</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="I27" s="1" t="n">
         <v>0.3258</v>
       </c>
-      <c r="F27" s="1" t="n">
+      <c r="J27" s="1" t="n">
         <v>0.2739</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>3019</v>
-      </c>
-      <c r="I27" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1358,29 +1358,29 @@
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="4" t="n">
+      <c r="C28" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>3020</v>
+      </c>
+      <c r="G28" s="4" t="n">
         <v>0.597</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="H28" s="1" t="n">
         <v>0.5656</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="I28" s="1" t="n">
         <v>0.3483</v>
       </c>
-      <c r="F28" s="1" t="n">
+      <c r="J28" s="1" t="n">
         <v>0.2959</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>3020</v>
-      </c>
-      <c r="I28" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,28 +1391,28 @@
         <v>45</v>
       </c>
       <c r="C29" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>3021</v>
+      </c>
+      <c r="G29" s="1" t="n">
         <v>0.5927</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="H29" s="1" t="n">
         <v>0.5626</v>
       </c>
-      <c r="E29" s="1" t="n">
+      <c r="I29" s="1" t="n">
         <v>0.3484</v>
       </c>
-      <c r="F29" s="1" t="n">
+      <c r="J29" s="1" t="n">
         <v>0.2958</v>
-      </c>
-      <c r="G29" s="1" t="n">
-        <v>3021</v>
-      </c>
-      <c r="I29" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1423,28 +1423,28 @@
         <v>46</v>
       </c>
       <c r="C30" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>3022</v>
+      </c>
+      <c r="G30" s="1" t="n">
         <v>0.6155</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="H30" s="1" t="n">
         <v>0.5856</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="I30" s="1" t="n">
         <v>0.3681</v>
       </c>
-      <c r="F30" s="1" t="n">
+      <c r="J30" s="1" t="n">
         <v>0.3099</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>3022</v>
-      </c>
-      <c r="I30" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,28 +1455,28 @@
         <v>47</v>
       </c>
       <c r="C31" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>3023</v>
+      </c>
+      <c r="G31" s="1" t="n">
         <v>0.5128</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="H31" s="1" t="n">
         <v>0.4823</v>
       </c>
-      <c r="E31" s="1" t="n">
+      <c r="I31" s="1" t="n">
         <v>0.2987</v>
       </c>
-      <c r="F31" s="4" t="n">
+      <c r="J31" s="4" t="n">
         <v>0.251</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>3023</v>
-      </c>
-      <c r="I31" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,28 +1487,28 @@
         <v>48</v>
       </c>
       <c r="C32" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>3024</v>
+      </c>
+      <c r="G32" s="1" t="n">
         <v>0.6009</v>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="H32" s="1" t="n">
         <v>0.5661</v>
       </c>
-      <c r="E32" s="1" t="n">
+      <c r="I32" s="1" t="n">
         <v>0.3565</v>
       </c>
-      <c r="F32" s="1" t="n">
+      <c r="J32" s="1" t="n">
         <v>0.2974</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>3024</v>
-      </c>
-      <c r="I32" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,29 +1518,29 @@
       <c r="B33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="4" t="n">
+      <c r="C33" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>3025</v>
+      </c>
+      <c r="G33" s="4" t="n">
         <v>0.537</v>
       </c>
-      <c r="D33" s="1" t="n">
+      <c r="H33" s="1" t="n">
         <v>0.5075</v>
       </c>
-      <c r="E33" s="1" t="n">
+      <c r="I33" s="1" t="n">
         <v>0.3131</v>
       </c>
-      <c r="F33" s="1" t="n">
+      <c r="J33" s="1" t="n">
         <v>0.2662</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>3025</v>
-      </c>
-      <c r="I33" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,28 +1551,28 @@
         <v>50</v>
       </c>
       <c r="C34" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>3026</v>
+      </c>
+      <c r="G34" s="1" t="n">
         <v>0.5782</v>
       </c>
-      <c r="D34" s="1" t="n">
+      <c r="H34" s="1" t="n">
         <v>0.5383</v>
       </c>
-      <c r="E34" s="1" t="n">
+      <c r="I34" s="1" t="n">
         <v>0.3393</v>
       </c>
-      <c r="F34" s="1" t="n">
+      <c r="J34" s="1" t="n">
         <v>0.2833</v>
-      </c>
-      <c r="G34" s="1" t="n">
-        <v>3026</v>
-      </c>
-      <c r="I34" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1583,28 +1583,28 @@
         <v>51</v>
       </c>
       <c r="C35" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>3027</v>
+      </c>
+      <c r="G35" s="1" t="n">
         <v>0.5304</v>
       </c>
-      <c r="D35" s="1" t="n">
+      <c r="H35" s="1" t="n">
         <v>0.4875</v>
       </c>
-      <c r="E35" s="1" t="n">
+      <c r="I35" s="1" t="n">
         <v>0.3037</v>
       </c>
-      <c r="F35" s="1" t="n">
+      <c r="J35" s="1" t="n">
         <v>0.2522</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>3027</v>
-      </c>
-      <c r="I35" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1615,28 +1615,28 @@
         <v>52</v>
       </c>
       <c r="C36" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>3028</v>
+      </c>
+      <c r="G36" s="1" t="n">
         <v>0.4571</v>
       </c>
-      <c r="D36" s="1" t="n">
+      <c r="H36" s="1" t="n">
         <v>0.4298</v>
       </c>
-      <c r="E36" s="1" t="n">
+      <c r="I36" s="1" t="n">
         <v>0.2663</v>
       </c>
-      <c r="F36" s="1" t="n">
+      <c r="J36" s="1" t="n">
         <v>0.2223</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <v>3028</v>
-      </c>
-      <c r="I36" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,29 +1646,29 @@
       <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="4" t="n">
+      <c r="C37" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>3029</v>
+      </c>
+      <c r="G37" s="4" t="n">
         <v>0.384</v>
       </c>
-      <c r="D37" s="1" t="n">
+      <c r="H37" s="1" t="n">
         <v>0.3494</v>
       </c>
-      <c r="E37" s="1" t="n">
+      <c r="I37" s="1" t="n">
         <v>0.2141</v>
       </c>
-      <c r="F37" s="1" t="n">
+      <c r="J37" s="1" t="n">
         <v>0.1735</v>
-      </c>
-      <c r="G37" s="1" t="n">
-        <v>3029</v>
-      </c>
-      <c r="I37" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,28 +1679,28 @@
         <v>54</v>
       </c>
       <c r="C38" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>3030</v>
+      </c>
+      <c r="G38" s="1" t="n">
         <v>0.5799</v>
       </c>
-      <c r="D38" s="1" t="n">
+      <c r="H38" s="1" t="n">
         <v>0.5477</v>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="I38" s="1" t="n">
         <v>0.3448</v>
       </c>
-      <c r="F38" s="1" t="n">
+      <c r="J38" s="1" t="n">
         <v>0.2901</v>
-      </c>
-      <c r="G38" s="1" t="n">
-        <v>3030</v>
-      </c>
-      <c r="I38" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,31 +1711,31 @@
         <v>55</v>
       </c>
       <c r="C39" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>3031</v>
+      </c>
+      <c r="G39" s="1" t="n">
         <v>0.5348</v>
       </c>
-      <c r="D39" s="1" t="n">
+      <c r="H39" s="1" t="n">
         <v>0.5079</v>
       </c>
-      <c r="E39" s="1" t="n">
+      <c r="I39" s="1" t="n">
         <v>0.3157</v>
       </c>
-      <c r="F39" s="1" t="n">
+      <c r="J39" s="1" t="n">
         <v>0.2674</v>
       </c>
-      <c r="G39" s="1" t="n">
-        <v>3031</v>
-      </c>
-      <c r="H39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I39" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,28 +1746,28 @@
         <v>56</v>
       </c>
       <c r="C40" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>3032</v>
+      </c>
+      <c r="G40" s="1" t="n">
         <v>0.6018</v>
       </c>
-      <c r="D40" s="1" t="n">
+      <c r="H40" s="1" t="n">
         <v>0.5687</v>
       </c>
-      <c r="E40" s="1" t="n">
+      <c r="I40" s="1" t="n">
         <v>0.3504</v>
       </c>
-      <c r="F40" s="1" t="n">
+      <c r="J40" s="1" t="n">
         <v>0.2975</v>
-      </c>
-      <c r="G40" s="1" t="n">
-        <v>3032</v>
-      </c>
-      <c r="I40" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1777,24 +1777,24 @@
       <c r="B41" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="4" t="n">
+      <c r="D41" s="4"/>
+      <c r="E41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>3033</v>
+      </c>
+      <c r="G41" s="4" t="n">
         <v>0.52</v>
       </c>
-      <c r="D41" s="1" t="n">
+      <c r="H41" s="1" t="n">
         <v>0.4797</v>
       </c>
-      <c r="E41" s="1" t="n">
+      <c r="I41" s="1" t="n">
         <v>0.2955</v>
       </c>
-      <c r="F41" s="1" t="n">
+      <c r="J41" s="1" t="n">
         <v>0.2488</v>
-      </c>
-      <c r="G41" s="1" t="n">
-        <v>3033</v>
-      </c>
-      <c r="J41" s="4"/>
-      <c r="K41" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,33 +1805,29 @@
         <v>58</v>
       </c>
       <c r="C42" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>3112</v>
+      </c>
+      <c r="G42" s="1" t="n">
         <v>0.5154</v>
       </c>
-      <c r="D42" s="1" t="n">
+      <c r="H42" s="1" t="n">
         <v>0.477</v>
       </c>
-      <c r="E42" s="1" t="n">
+      <c r="I42" s="1" t="n">
         <v>0.3031</v>
       </c>
-      <c r="F42" s="1" t="n">
+      <c r="J42" s="1" t="n">
         <v>0.2561</v>
       </c>
-      <c r="G42" s="1" t="n">
-        <v>3112</v>
-      </c>
-      <c r="I42" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
@@ -1867,6 +1863,10 @@
       <c r="AW42" s="1"/>
       <c r="AX42" s="1"/>
       <c r="AY42" s="1"/>
+      <c r="AZ42" s="1"/>
+      <c r="BA42" s="1"/>
+      <c r="BB42" s="1"/>
+      <c r="BC42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -1876,28 +1876,28 @@
         <v>59</v>
       </c>
       <c r="C43" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>3105</v>
+      </c>
+      <c r="G43" s="1" t="n">
         <v>0.5808</v>
       </c>
-      <c r="D43" s="1" t="n">
+      <c r="H43" s="1" t="n">
         <v>0.5437</v>
       </c>
-      <c r="E43" s="1" t="n">
+      <c r="I43" s="1" t="n">
         <v>0.3444</v>
       </c>
-      <c r="F43" s="1" t="n">
+      <c r="J43" s="1" t="n">
         <v>0.2898</v>
-      </c>
-      <c r="G43" s="1" t="n">
-        <v>3105</v>
-      </c>
-      <c r="I43" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,28 +1908,28 @@
         <v>60</v>
       </c>
       <c r="C44" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>3106</v>
+      </c>
+      <c r="G44" s="1" t="n">
         <v>0.5297</v>
       </c>
-      <c r="D44" s="1" t="n">
+      <c r="H44" s="1" t="n">
         <v>0.4877</v>
       </c>
-      <c r="E44" s="1" t="n">
+      <c r="I44" s="1" t="n">
         <v>0.3094</v>
       </c>
-      <c r="F44" s="1" t="n">
+      <c r="J44" s="1" t="n">
         <v>0.2552</v>
-      </c>
-      <c r="G44" s="1" t="n">
-        <v>3106</v>
-      </c>
-      <c r="I44" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,28 +1940,28 @@
         <v>61</v>
       </c>
       <c r="C45" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>3107</v>
+      </c>
+      <c r="G45" s="1" t="n">
         <v>0.6231</v>
       </c>
-      <c r="D45" s="1" t="n">
+      <c r="H45" s="1" t="n">
         <v>0.5822</v>
       </c>
-      <c r="E45" s="1" t="n">
+      <c r="I45" s="1" t="n">
         <v>0.3673</v>
       </c>
-      <c r="F45" s="1" t="n">
+      <c r="J45" s="1" t="n">
         <v>0.3105</v>
-      </c>
-      <c r="G45" s="1" t="n">
-        <v>3107</v>
-      </c>
-      <c r="I45" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,28 +1972,28 @@
         <v>62</v>
       </c>
       <c r="C46" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>3108</v>
+      </c>
+      <c r="G46" s="1" t="n">
         <v>0.5526</v>
       </c>
-      <c r="D46" s="1" t="n">
+      <c r="H46" s="1" t="n">
         <v>0.5148</v>
       </c>
-      <c r="E46" s="1" t="n">
+      <c r="I46" s="1" t="n">
         <v>0.3313</v>
       </c>
-      <c r="F46" s="1" t="n">
+      <c r="J46" s="1" t="n">
         <v>0.2774</v>
-      </c>
-      <c r="G46" s="1" t="n">
-        <v>3108</v>
-      </c>
-      <c r="I46" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,28 +2004,28 @@
         <v>63</v>
       </c>
       <c r="C47" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>3109</v>
+      </c>
+      <c r="G47" s="1" t="n">
         <v>0.6166</v>
       </c>
-      <c r="D47" s="1" t="n">
+      <c r="H47" s="1" t="n">
         <v>0.5782</v>
       </c>
-      <c r="E47" s="1" t="n">
+      <c r="I47" s="1" t="n">
         <v>0.3711</v>
       </c>
-      <c r="F47" s="1" t="n">
+      <c r="J47" s="1" t="n">
         <v>0.3092</v>
-      </c>
-      <c r="G47" s="1" t="n">
-        <v>3109</v>
-      </c>
-      <c r="I47" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2036,31 +2036,31 @@
         <v>64</v>
       </c>
       <c r="C48" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>3110</v>
+      </c>
+      <c r="G48" s="1" t="n">
         <v>0.616</v>
       </c>
-      <c r="D48" s="1" t="n">
+      <c r="H48" s="1" t="n">
         <v>0.5753</v>
       </c>
-      <c r="E48" s="1" t="n">
+      <c r="I48" s="1" t="n">
         <v>0.369</v>
       </c>
-      <c r="F48" s="1" t="n">
+      <c r="J48" s="1" t="n">
         <v>0.3052</v>
       </c>
-      <c r="G48" s="1" t="n">
-        <v>3110</v>
-      </c>
-      <c r="H48" s="1" t="s">
+      <c r="K48" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I48" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2071,28 +2071,28 @@
         <v>65</v>
       </c>
       <c r="C49" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>3111</v>
+      </c>
+      <c r="G49" s="1" t="n">
         <v>0.6012</v>
       </c>
-      <c r="D49" s="1" t="n">
+      <c r="H49" s="1" t="n">
         <v>0.5604</v>
       </c>
-      <c r="E49" s="1" t="n">
+      <c r="I49" s="1" t="n">
         <v>0.3488</v>
       </c>
-      <c r="F49" s="1" t="n">
+      <c r="J49" s="1" t="n">
         <v>0.2932</v>
-      </c>
-      <c r="G49" s="1" t="n">
-        <v>3111</v>
-      </c>
-      <c r="I49" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2103,28 +2103,28 @@
         <v>66</v>
       </c>
       <c r="C50" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>3102</v>
+      </c>
+      <c r="G50" s="1" t="n">
         <v>0.6259</v>
       </c>
-      <c r="D50" s="1" t="n">
+      <c r="H50" s="1" t="n">
         <v>0.5893</v>
       </c>
-      <c r="E50" s="1" t="n">
+      <c r="I50" s="1" t="n">
         <v>0.3735</v>
       </c>
-      <c r="F50" s="1" t="n">
+      <c r="J50" s="1" t="n">
         <v>0.3136</v>
-      </c>
-      <c r="G50" s="1" t="n">
-        <v>3102</v>
-      </c>
-      <c r="I50" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2135,28 +2135,28 @@
         <v>67</v>
       </c>
       <c r="C51" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>3103</v>
+      </c>
+      <c r="G51" s="1" t="n">
         <v>0.4081</v>
       </c>
-      <c r="D51" s="1" t="n">
+      <c r="H51" s="1" t="n">
         <v>0.3472</v>
       </c>
-      <c r="E51" s="1" t="n">
+      <c r="I51" s="1" t="n">
         <v>0.2161</v>
       </c>
-      <c r="F51" s="1" t="n">
+      <c r="J51" s="1" t="n">
         <v>0.182</v>
-      </c>
-      <c r="G51" s="1" t="n">
-        <v>3103</v>
-      </c>
-      <c r="I51" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2167,28 +2167,28 @@
         <v>68</v>
       </c>
       <c r="C52" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>3104</v>
+      </c>
+      <c r="G52" s="1" t="n">
         <v>0.6034</v>
       </c>
-      <c r="D52" s="1" t="n">
+      <c r="H52" s="1" t="n">
         <v>0.567</v>
       </c>
-      <c r="E52" s="1" t="n">
+      <c r="I52" s="1" t="n">
         <v>0.367</v>
       </c>
-      <c r="F52" s="1" t="n">
+      <c r="J52" s="1" t="n">
         <v>0.3046</v>
-      </c>
-      <c r="G52" s="1" t="n">
-        <v>3104</v>
-      </c>
-      <c r="I52" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2199,28 +2199,28 @@
         <v>69</v>
       </c>
       <c r="C53" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>3095</v>
+      </c>
+      <c r="G53" s="1" t="n">
         <v>0.558</v>
       </c>
-      <c r="D53" s="1" t="n">
+      <c r="H53" s="1" t="n">
         <v>0.5194</v>
       </c>
-      <c r="E53" s="1" t="n">
+      <c r="I53" s="1" t="n">
         <v>0.3298</v>
       </c>
-      <c r="F53" s="1" t="n">
+      <c r="J53" s="1" t="n">
         <v>0.2756</v>
-      </c>
-      <c r="G53" s="1" t="n">
-        <v>3095</v>
-      </c>
-      <c r="I53" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,28 +2231,28 @@
         <v>70</v>
       </c>
       <c r="C54" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>3096</v>
+      </c>
+      <c r="G54" s="1" t="n">
         <v>0.5753</v>
       </c>
-      <c r="D54" s="1" t="n">
+      <c r="H54" s="1" t="n">
         <v>0.5326</v>
       </c>
-      <c r="E54" s="1" t="n">
+      <c r="I54" s="1" t="n">
         <v>0.3372</v>
       </c>
-      <c r="F54" s="1" t="n">
+      <c r="J54" s="1" t="n">
         <v>0.2835</v>
-      </c>
-      <c r="G54" s="1" t="n">
-        <v>3096</v>
-      </c>
-      <c r="I54" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="J54" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,28 +2263,28 @@
         <v>71</v>
       </c>
       <c r="C55" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>3097</v>
+      </c>
+      <c r="G55" s="1" t="n">
         <v>0.5093</v>
       </c>
-      <c r="D55" s="1" t="n">
+      <c r="H55" s="1" t="n">
         <v>0.4568</v>
       </c>
-      <c r="E55" s="1" t="n">
+      <c r="I55" s="1" t="n">
         <v>0.2881</v>
       </c>
-      <c r="F55" s="1" t="n">
+      <c r="J55" s="1" t="n">
         <v>0.2401</v>
-      </c>
-      <c r="G55" s="1" t="n">
-        <v>3097</v>
-      </c>
-      <c r="I55" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,28 +2295,28 @@
         <v>72</v>
       </c>
       <c r="C56" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>3098</v>
+      </c>
+      <c r="G56" s="1" t="n">
         <v>0.543</v>
       </c>
-      <c r="D56" s="1" t="n">
+      <c r="H56" s="1" t="n">
         <v>0.4991</v>
       </c>
-      <c r="E56" s="1" t="n">
+      <c r="I56" s="1" t="n">
         <v>0.3079</v>
       </c>
-      <c r="F56" s="1" t="n">
+      <c r="J56" s="1" t="n">
         <v>0.2635</v>
-      </c>
-      <c r="G56" s="1" t="n">
-        <v>3098</v>
-      </c>
-      <c r="I56" s="1" t="n">
-        <v>84</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2327,28 +2327,28 @@
         <v>73</v>
       </c>
       <c r="C57" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" s="1" t="n">
+        <v>3099</v>
+      </c>
+      <c r="G57" s="1" t="n">
         <v>0.6157</v>
       </c>
-      <c r="D57" s="1" t="n">
+      <c r="H57" s="1" t="n">
         <v>0.571</v>
       </c>
-      <c r="E57" s="1" t="n">
+      <c r="I57" s="1" t="n">
         <v>0.3564</v>
       </c>
-      <c r="F57" s="1" t="n">
+      <c r="J57" s="1" t="n">
         <v>0.3041</v>
-      </c>
-      <c r="G57" s="1" t="n">
-        <v>3099</v>
-      </c>
-      <c r="I57" s="1" t="n">
-        <v>84</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,28 +2359,28 @@
         <v>74</v>
       </c>
       <c r="C58" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <v>3100</v>
+      </c>
+      <c r="G58" s="1" t="n">
         <v>0.5963</v>
       </c>
-      <c r="D58" s="1" t="n">
+      <c r="H58" s="1" t="n">
         <v>0.5548</v>
       </c>
-      <c r="E58" s="1" t="n">
+      <c r="I58" s="1" t="n">
         <v>0.3537</v>
       </c>
-      <c r="F58" s="1" t="n">
+      <c r="J58" s="1" t="n">
         <v>0.2963</v>
-      </c>
-      <c r="G58" s="1" t="n">
-        <v>3100</v>
-      </c>
-      <c r="I58" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2391,31 +2391,31 @@
         <v>75</v>
       </c>
       <c r="C59" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>3101</v>
+      </c>
+      <c r="G59" s="1" t="n">
         <v>0.6115</v>
       </c>
-      <c r="D59" s="1" t="n">
+      <c r="H59" s="1" t="n">
         <v>0.5764</v>
       </c>
-      <c r="E59" s="1" t="n">
+      <c r="I59" s="1" t="n">
         <v>0.3638</v>
       </c>
-      <c r="F59" s="1" t="n">
+      <c r="J59" s="1" t="n">
         <v>0.3073</v>
       </c>
-      <c r="G59" s="1" t="n">
-        <v>3101</v>
-      </c>
-      <c r="H59" s="1" t="s">
+      <c r="K59" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I59" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2426,31 +2426,31 @@
         <v>76</v>
       </c>
       <c r="C60" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="1" t="n">
+        <v>3093</v>
+      </c>
+      <c r="G60" s="1" t="n">
         <v>0.62</v>
       </c>
-      <c r="D60" s="1" t="n">
+      <c r="H60" s="1" t="n">
         <v>0.5826</v>
       </c>
-      <c r="E60" s="1" t="n">
+      <c r="I60" s="1" t="n">
         <v>0.3675</v>
       </c>
-      <c r="F60" s="1" t="n">
+      <c r="J60" s="1" t="n">
         <v>0.3114</v>
       </c>
-      <c r="G60" s="1" t="n">
-        <v>3093</v>
-      </c>
-      <c r="H60" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I60" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2461,28 +2461,28 @@
         <v>77</v>
       </c>
       <c r="C61" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="1" t="n">
+        <v>3094</v>
+      </c>
+      <c r="G61" s="1" t="n">
         <v>0.5576</v>
       </c>
-      <c r="D61" s="1" t="n">
+      <c r="H61" s="1" t="n">
         <v>0.521</v>
       </c>
-      <c r="E61" s="1" t="n">
+      <c r="I61" s="1" t="n">
         <v>0.3264</v>
       </c>
-      <c r="F61" s="1" t="n">
+      <c r="J61" s="1" t="n">
         <v>0.275</v>
-      </c>
-      <c r="G61" s="1" t="n">
-        <v>3094</v>
-      </c>
-      <c r="I61" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,28 +2493,28 @@
         <v>78</v>
       </c>
       <c r="C62" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="1" t="n">
+        <v>3092</v>
+      </c>
+      <c r="G62" s="1" t="n">
         <v>0.5735</v>
       </c>
-      <c r="D62" s="1" t="n">
+      <c r="H62" s="1" t="n">
         <v>0.535</v>
       </c>
-      <c r="E62" s="1" t="n">
+      <c r="I62" s="1" t="n">
         <v>0.3299</v>
       </c>
-      <c r="F62" s="1" t="n">
+      <c r="J62" s="1" t="n">
         <v>0.2825</v>
-      </c>
-      <c r="G62" s="1" t="n">
-        <v>3092</v>
-      </c>
-      <c r="I62" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,28 +2525,28 @@
         <v>79</v>
       </c>
       <c r="C63" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" s="1" t="n">
+        <v>3088</v>
+      </c>
+      <c r="G63" s="1" t="n">
         <v>0.6063</v>
       </c>
-      <c r="D63" s="1" t="n">
+      <c r="H63" s="1" t="n">
         <v>0.5683</v>
       </c>
-      <c r="E63" s="1" t="n">
+      <c r="I63" s="1" t="n">
         <v>0.3523</v>
       </c>
-      <c r="F63" s="1" t="n">
+      <c r="J63" s="1" t="n">
         <v>0.2989</v>
-      </c>
-      <c r="G63" s="1" t="n">
-        <v>3088</v>
-      </c>
-      <c r="I63" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2557,28 +2557,28 @@
         <v>80</v>
       </c>
       <c r="C64" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="1" t="n">
+        <v>3089</v>
+      </c>
+      <c r="G64" s="1" t="n">
         <v>0.5711</v>
       </c>
-      <c r="D64" s="1" t="n">
+      <c r="H64" s="1" t="n">
         <v>0.5341</v>
       </c>
-      <c r="E64" s="1" t="n">
+      <c r="I64" s="1" t="n">
         <v>0.335</v>
       </c>
-      <c r="F64" s="1" t="n">
+      <c r="J64" s="1" t="n">
         <v>0.2842</v>
-      </c>
-      <c r="G64" s="1" t="n">
-        <v>3089</v>
-      </c>
-      <c r="I64" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2589,28 +2589,28 @@
         <v>81</v>
       </c>
       <c r="C65" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="1" t="n">
+        <v>3090</v>
+      </c>
+      <c r="G65" s="1" t="n">
         <v>0.5817</v>
       </c>
-      <c r="D65" s="1" t="n">
+      <c r="H65" s="1" t="n">
         <v>0.5458</v>
       </c>
-      <c r="E65" s="1" t="n">
+      <c r="I65" s="1" t="n">
         <v>0.3416</v>
       </c>
-      <c r="F65" s="1" t="n">
+      <c r="J65" s="1" t="n">
         <v>0.288</v>
-      </c>
-      <c r="G65" s="1" t="n">
-        <v>3090</v>
-      </c>
-      <c r="I65" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K65" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2621,28 +2621,28 @@
         <v>82</v>
       </c>
       <c r="C66" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="1" t="n">
+        <v>3091</v>
+      </c>
+      <c r="G66" s="1" t="n">
         <v>0.5617</v>
       </c>
-      <c r="D66" s="1" t="n">
+      <c r="H66" s="1" t="n">
         <v>0.5227</v>
       </c>
-      <c r="E66" s="1" t="n">
+      <c r="I66" s="1" t="n">
         <v>0.3285</v>
       </c>
-      <c r="F66" s="1" t="n">
+      <c r="J66" s="1" t="n">
         <v>0.2775</v>
-      </c>
-      <c r="G66" s="1" t="n">
-        <v>3091</v>
-      </c>
-      <c r="I66" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="J66" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,28 +2653,28 @@
         <v>83</v>
       </c>
       <c r="C67" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" s="1" t="n">
+        <v>3081</v>
+      </c>
+      <c r="G67" s="1" t="n">
         <v>0.5667</v>
       </c>
-      <c r="D67" s="1" t="n">
+      <c r="H67" s="1" t="n">
         <v>0.528</v>
       </c>
-      <c r="E67" s="1" t="n">
+      <c r="I67" s="1" t="n">
         <v>0.3313</v>
       </c>
-      <c r="F67" s="1" t="n">
+      <c r="J67" s="1" t="n">
         <v>0.2801</v>
-      </c>
-      <c r="G67" s="1" t="n">
-        <v>3081</v>
-      </c>
-      <c r="I67" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="J67" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K67" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,28 +2685,28 @@
         <v>84</v>
       </c>
       <c r="C68" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" s="1" t="n">
+        <v>3082</v>
+      </c>
+      <c r="G68" s="1" t="n">
         <v>0.5488</v>
       </c>
-      <c r="D68" s="1" t="n">
+      <c r="H68" s="1" t="n">
         <v>0.5045</v>
       </c>
-      <c r="E68" s="1" t="n">
+      <c r="I68" s="1" t="n">
         <v>0.3138</v>
       </c>
-      <c r="F68" s="1" t="n">
+      <c r="J68" s="1" t="n">
         <v>0.2648</v>
-      </c>
-      <c r="G68" s="1" t="n">
-        <v>3082</v>
-      </c>
-      <c r="I68" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="J68" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K68" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,28 +2717,28 @@
         <v>85</v>
       </c>
       <c r="C69" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" s="1" t="n">
+        <v>3083</v>
+      </c>
+      <c r="G69" s="1" t="n">
         <v>0.5118</v>
       </c>
-      <c r="D69" s="1" t="n">
+      <c r="H69" s="1" t="n">
         <v>0.474</v>
       </c>
-      <c r="E69" s="1" t="n">
+      <c r="I69" s="1" t="n">
         <v>0.2975</v>
       </c>
-      <c r="F69" s="1" t="n">
+      <c r="J69" s="1" t="n">
         <v>0.2436</v>
-      </c>
-      <c r="G69" s="1" t="n">
-        <v>3083</v>
-      </c>
-      <c r="I69" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="J69" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K69" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2749,28 +2749,28 @@
         <v>86</v>
       </c>
       <c r="C70" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="1" t="n">
+        <v>3084</v>
+      </c>
+      <c r="G70" s="1" t="n">
         <v>0.4949</v>
       </c>
-      <c r="D70" s="1" t="n">
+      <c r="H70" s="1" t="n">
         <v>0.472</v>
       </c>
-      <c r="E70" s="1" t="n">
+      <c r="I70" s="1" t="n">
         <v>0.3028</v>
       </c>
-      <c r="F70" s="1" t="n">
+      <c r="J70" s="1" t="n">
         <v>0.2537</v>
-      </c>
-      <c r="G70" s="1" t="n">
-        <v>3084</v>
-      </c>
-      <c r="I70" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K70" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2781,28 +2781,28 @@
         <v>87</v>
       </c>
       <c r="C71" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" s="1" t="n">
+        <v>3085</v>
+      </c>
+      <c r="G71" s="1" t="n">
         <v>0.5966</v>
       </c>
-      <c r="D71" s="1" t="n">
+      <c r="H71" s="1" t="n">
         <v>0.5683</v>
       </c>
-      <c r="E71" s="1" t="n">
+      <c r="I71" s="1" t="n">
         <v>0.3653</v>
       </c>
-      <c r="F71" s="1" t="n">
+      <c r="J71" s="1" t="n">
         <v>0.3057</v>
-      </c>
-      <c r="G71" s="1" t="n">
-        <v>3085</v>
-      </c>
-      <c r="I71" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="J71" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K71" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2813,28 +2813,28 @@
         <v>88</v>
       </c>
       <c r="C72" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="1" t="n">
+        <v>3074</v>
+      </c>
+      <c r="G72" s="1" t="n">
         <v>0.5994</v>
       </c>
-      <c r="D72" s="1" t="n">
+      <c r="H72" s="1" t="n">
         <v>0.571</v>
       </c>
-      <c r="E72" s="1" t="n">
+      <c r="I72" s="1" t="n">
         <v>0.3626</v>
       </c>
-      <c r="F72" s="1" t="n">
+      <c r="J72" s="1" t="n">
         <v>0.3024</v>
-      </c>
-      <c r="G72" s="1" t="n">
-        <v>3074</v>
-      </c>
-      <c r="I72" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K72" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2845,31 +2845,31 @@
         <v>89</v>
       </c>
       <c r="C73" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F73" s="1" t="n">
+        <v>3075</v>
+      </c>
+      <c r="G73" s="1" t="n">
         <v>0.5666</v>
       </c>
-      <c r="D73" s="1" t="n">
+      <c r="H73" s="1" t="n">
         <v>0.5414</v>
       </c>
-      <c r="E73" s="1" t="n">
+      <c r="I73" s="1" t="n">
         <v>0.3379</v>
       </c>
-      <c r="F73" s="1" t="n">
+      <c r="J73" s="1" t="n">
         <v>0.2815</v>
       </c>
-      <c r="G73" s="1" t="n">
-        <v>3075</v>
-      </c>
-      <c r="H73" s="1" t="s">
+      <c r="K73" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="I73" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K73" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2880,28 +2880,28 @@
         <v>91</v>
       </c>
       <c r="C74" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F74" s="1" t="n">
+        <v>3076</v>
+      </c>
+      <c r="G74" s="1" t="n">
         <v>0.5385</v>
       </c>
-      <c r="D74" s="1" t="n">
+      <c r="H74" s="1" t="n">
         <v>0.5115</v>
       </c>
-      <c r="E74" s="1" t="n">
+      <c r="I74" s="1" t="n">
         <v>0.3227</v>
       </c>
-      <c r="F74" s="1" t="n">
+      <c r="J74" s="1" t="n">
         <v>0.27</v>
-      </c>
-      <c r="G74" s="1" t="n">
-        <v>3076</v>
-      </c>
-      <c r="I74" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="J74" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2912,28 +2912,28 @@
         <v>92</v>
       </c>
       <c r="C75" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F75" s="1" t="n">
+        <v>3079</v>
+      </c>
+      <c r="G75" s="1" t="n">
         <v>0.5566</v>
       </c>
-      <c r="D75" s="1" t="n">
+      <c r="H75" s="1" t="n">
         <v>0.5293</v>
       </c>
-      <c r="E75" s="1" t="n">
+      <c r="I75" s="1" t="n">
         <v>0.3292</v>
       </c>
-      <c r="F75" s="1" t="n">
+      <c r="J75" s="1" t="n">
         <v>0.2788</v>
-      </c>
-      <c r="G75" s="1" t="n">
-        <v>3079</v>
-      </c>
-      <c r="I75" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K75" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2944,28 +2944,28 @@
         <v>93</v>
       </c>
       <c r="C76" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" s="1" t="n">
+        <v>3080</v>
+      </c>
+      <c r="G76" s="1" t="n">
         <v>0.5749</v>
       </c>
-      <c r="D76" s="1" t="n">
+      <c r="H76" s="1" t="n">
         <v>0.5444</v>
       </c>
-      <c r="E76" s="1" t="n">
+      <c r="I76" s="1" t="n">
         <v>0.3376</v>
       </c>
-      <c r="F76" s="1" t="n">
+      <c r="J76" s="1" t="n">
         <v>0.2828</v>
-      </c>
-      <c r="G76" s="1" t="n">
-        <v>3080</v>
-      </c>
-      <c r="I76" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2976,28 +2976,28 @@
         <v>94</v>
       </c>
       <c r="C77" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F77" s="1" t="n">
+        <v>3071</v>
+      </c>
+      <c r="G77" s="1" t="n">
         <v>0.5927</v>
       </c>
-      <c r="D77" s="1" t="n">
+      <c r="H77" s="1" t="n">
         <v>0.5678</v>
       </c>
-      <c r="E77" s="1" t="n">
+      <c r="I77" s="1" t="n">
         <v>0.3605</v>
       </c>
-      <c r="F77" s="1" t="n">
+      <c r="J77" s="1" t="n">
         <v>0.3035</v>
-      </c>
-      <c r="G77" s="1" t="n">
-        <v>3071</v>
-      </c>
-      <c r="I77" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,31 +3008,31 @@
         <v>95</v>
       </c>
       <c r="C78" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" s="1" t="n">
+        <v>3072</v>
+      </c>
+      <c r="G78" s="1" t="n">
         <v>0.5992</v>
       </c>
-      <c r="D78" s="1" t="n">
+      <c r="H78" s="1" t="n">
         <v>0.5699</v>
       </c>
-      <c r="E78" s="1" t="n">
+      <c r="I78" s="1" t="n">
         <v>0.3577</v>
       </c>
-      <c r="F78" s="1" t="n">
+      <c r="J78" s="1" t="n">
         <v>0.3003</v>
       </c>
-      <c r="G78" s="1" t="n">
-        <v>3072</v>
-      </c>
-      <c r="H78" s="1" t="s">
+      <c r="K78" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="I78" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="J78" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K78" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3043,28 +3043,28 @@
         <v>96</v>
       </c>
       <c r="C79" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F79" s="1" t="n">
+        <v>3073</v>
+      </c>
+      <c r="G79" s="1" t="n">
         <v>0.5788</v>
       </c>
-      <c r="D79" s="1" t="n">
+      <c r="H79" s="1" t="n">
         <v>0.5522</v>
       </c>
-      <c r="E79" s="1" t="n">
+      <c r="I79" s="1" t="n">
         <v>0.3489</v>
       </c>
-      <c r="F79" s="1" t="n">
+      <c r="J79" s="1" t="n">
         <v>0.2899</v>
-      </c>
-      <c r="G79" s="1" t="n">
-        <v>3073</v>
-      </c>
-      <c r="I79" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="J79" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K79" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3075,28 +3075,28 @@
         <v>97</v>
       </c>
       <c r="C80" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="1" t="n">
+        <v>3077</v>
+      </c>
+      <c r="G80" s="1" t="n">
         <v>0.5113</v>
       </c>
-      <c r="D80" s="1" t="n">
+      <c r="H80" s="1" t="n">
         <v>0.4856</v>
       </c>
-      <c r="E80" s="1" t="n">
+      <c r="I80" s="1" t="n">
         <v>0.3094</v>
       </c>
-      <c r="F80" s="1" t="n">
+      <c r="J80" s="1" t="n">
         <v>0.2593</v>
-      </c>
-      <c r="G80" s="1" t="n">
-        <v>3077</v>
-      </c>
-      <c r="I80" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="J80" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3107,28 +3107,28 @@
         <v>98</v>
       </c>
       <c r="C81" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <v>3078</v>
+      </c>
+      <c r="G81" s="1" t="n">
         <v>0.577</v>
       </c>
-      <c r="D81" s="1" t="n">
+      <c r="H81" s="1" t="n">
         <v>0.5491</v>
       </c>
-      <c r="E81" s="1" t="n">
+      <c r="I81" s="1" t="n">
         <v>0.34</v>
       </c>
-      <c r="F81" s="1" t="n">
+      <c r="J81" s="1" t="n">
         <v>0.2907</v>
-      </c>
-      <c r="G81" s="1" t="n">
-        <v>3078</v>
-      </c>
-      <c r="I81" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K81" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>